<commit_message>
Fixed transect error in Baker South, 2014, Transect 2 - had been mislabeled as transect 3 in quads
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2014/Baker South Entry 2014/Baker South Quads 2014.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2014/Baker South Entry 2014/Baker South Quads 2014.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14640"/>
+    <workbookView xWindow="400" yWindow="1640" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -1338,15 +1338,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1586,7 +1582,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1979,15 +1975,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1014"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="9.1640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" style="6" customWidth="1"/>
@@ -2937,7 +2933,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>17</v>
@@ -2993,7 +2989,7 @@
         <v>24</v>
       </c>
       <c r="F20" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>18</v>
@@ -3049,7 +3045,7 @@
         <v>24</v>
       </c>
       <c r="F21" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>3</v>
@@ -3107,7 +3103,7 @@
         <v>24</v>
       </c>
       <c r="F22" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>48</v>
@@ -3165,7 +3161,7 @@
         <v>24</v>
       </c>
       <c r="F23" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>21</v>
@@ -3217,7 +3213,7 @@
         <v>24</v>
       </c>
       <c r="F24" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>160</v>
@@ -5385,7 +5381,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G119:G129 X2:X7 G33:G80 G18 G10 G25 G131:G138 G105:G117 G86:G91 G93:G102">
@@ -5414,7 +5409,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -5422,14 +5417,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="16"/>
   </cols>
@@ -6094,7 +6089,7 @@
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>